<commit_message>
Update TP1 Canvas2 and titles
</commit_message>
<xml_diff>
--- a/canvas/Canvas TP 2.xlsx
+++ b/canvas/Canvas TP 2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -85,22 +85,22 @@
     <t>Utilisation de smart contract</t>
   </si>
   <si>
-    <t>Ceux qui émettent les actions et ceux qui les achètent / les possèdent</t>
-  </si>
-  <si>
-    <t>Ceux qui participent souhaitent de la transparence dans la répartition des actions</t>
-  </si>
-  <si>
-    <t>Avoir une vue claire et précise des différents actionnaires de l'entreprise</t>
-  </si>
-  <si>
-    <t>Gestion des actions d'une entreprise</t>
-  </si>
-  <si>
-    <t>Tout le monde peut consulter les données mais seuls les utilisateurs enregistrés peuvent acheter ou vendre des actions</t>
-  </si>
-  <si>
-    <t>Les acteurs peuvent acheter des actions si il y a de la disponibilité et peuvent aussi les mettre en vente</t>
+    <t>Points de fidélité et monnaie locale</t>
+  </si>
+  <si>
+    <t>Ceux qui émettent les points de fidélité et ceux qui les recoivent</t>
+  </si>
+  <si>
+    <t>Ceux qui participent souhaitent de la transparence dans la répartition des points de fidélité</t>
+  </si>
+  <si>
+    <t>Avoir une vue claire et précise des différents points de fidélité accordés</t>
+  </si>
+  <si>
+    <t>Tout le monde peut consulter les données mais seuls les utilisateurs enregistrés peuvent bénéficier des points de fidélité et de la monnaie associée</t>
+  </si>
+  <si>
+    <t>Les acteurs peuvent bénéficier de points de fidélité qui seront transformés en monnaie locale</t>
   </si>
 </sst>
 </file>
@@ -702,7 +702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -740,16 +740,16 @@
     </row>
     <row r="3" spans="1:6" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>

</xml_diff>